<commit_message>
Encabezado Datos Personales y reduccion de código inicia
</commit_message>
<xml_diff>
--- a/FormatoPF.xlsx
+++ b/FormatoPF.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="121">
   <si>
     <t>E N C A B E Z A D O</t>
   </si>
@@ -308,13 +308,82 @@
   </si>
   <si>
     <t>Dias vencimiento</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>1qds</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>1234567890111</t>
+  </si>
+  <si>
+    <t>niña</t>
+  </si>
+  <si>
+    <t>adicional</t>
+  </si>
+  <si>
+    <t>Luz</t>
+  </si>
+  <si>
+    <t>dsa</t>
+  </si>
+  <si>
+    <t>asdj</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>Hola</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>clave1</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>corona</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>asdas</t>
+  </si>
+  <si>
+    <t>clave2</t>
+  </si>
+  <si>
+    <t>a veces</t>
+  </si>
+  <si>
+    <t>LA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +400,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -420,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,6 +517,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -738,7 +825,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU2"/>
+  <dimension ref="A1:CU5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -756,7 +843,7 @@
     <col min="10" max="10" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1257,6 +1344,156 @@
         <v>84</v>
       </c>
     </row>
+    <row r="3" spans="1:99">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="11">
+        <v>28042003</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="12">
+        <v>1012003</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" s="10">
+        <v>123</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="P3" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="U3" s="10">
+        <v>12</v>
+      </c>
+      <c r="V3" s="10">
+        <v>30061976</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:99">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11">
+        <v>2</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="N4" s="10">
+        <v>456</v>
+      </c>
+      <c r="O4" s="12"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:99">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:F1"/>

</xml_diff>

<commit_message>
Finalizar primera version de formato FM
</commit_message>
<xml_diff>
--- a/FormatoPF.xlsx
+++ b/FormatoPF.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="168">
   <si>
     <t>E N C A B E Z A D O</t>
   </si>
@@ -449,6 +449,81 @@
   </si>
   <si>
     <t>tres</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>zx</t>
+  </si>
+  <si>
+    <t>jk</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>ABCDEFG12345kkkkkkkkkkkkkkkkkk
+kAAAAAAAAAAAAAAAAAAAAAAAAAAAAA
+AAAAAAAAAAAAAAAAAAAAAAAAAAAAAA
+AAAAAAAAaaaaaaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>AAAAAAAAAAAAAAAAAAAAAAAAAAAAAA
+AAAAAAAAAAAAAAAAAAAAAAAAAAAAAA
+AAAAA</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>nombre1</t>
+  </si>
+  <si>
+    <t>correo@gmail.com</t>
+  </si>
+  <si>
+    <t>cde456</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>nombre2</t>
+  </si>
+  <si>
+    <t>name3</t>
+  </si>
+  <si>
+    <t>nombre3</t>
+  </si>
+  <si>
+    <t>Arturo</t>
+  </si>
+  <si>
+    <t>Mi domicilio muy largo para
+comprobar el salto de linea</t>
+  </si>
+  <si>
+    <t>Arturito</t>
   </si>
 </sst>
 </file>
@@ -971,14 +1046,14 @@
     <col min="66" max="66" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="21.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1001,7 +1076,7 @@
     <col min="96" max="96" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:99" s="1" customFormat="1">
@@ -1567,6 +1642,147 @@
       <c r="AZ3" s="10" t="s">
         <v>137</v>
       </c>
+      <c r="BA3" s="12">
+        <v>1234567890</v>
+      </c>
+      <c r="BB3" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="BC3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="BD3" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="BE3" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="BF3" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="BG3" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="BH3" s="10">
+        <v>123456789</v>
+      </c>
+      <c r="BI3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="BJ3" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="BK3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="BL3" s="11">
+        <v>5112023</v>
+      </c>
+      <c r="BM3" s="11">
+        <v>18032024</v>
+      </c>
+      <c r="BN3" s="11">
+        <v>29092022</v>
+      </c>
+      <c r="BO3" s="10">
+        <v>7082023</v>
+      </c>
+      <c r="BP3" s="11">
+        <v>5112023</v>
+      </c>
+      <c r="BQ3" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="BR3" s="11">
+        <v>1234</v>
+      </c>
+      <c r="BS3" s="11">
+        <v>1234567890</v>
+      </c>
+      <c r="BT3" s="11">
+        <v>123456789</v>
+      </c>
+      <c r="BU3" s="11">
+        <v>123456789</v>
+      </c>
+      <c r="BV3" s="10">
+        <v>1234</v>
+      </c>
+      <c r="BW3" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="BX3" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY3" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="BZ3" s="10">
+        <v>123</v>
+      </c>
+      <c r="CA3" s="10">
+        <v>1234567890</v>
+      </c>
+      <c r="CB3" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="CC3" s="10">
+        <v>1234567890</v>
+      </c>
+      <c r="CD3" s="12">
+        <v>27042006</v>
+      </c>
+      <c r="CE3" s="11">
+        <v>1234567890</v>
+      </c>
+      <c r="CF3" s="12">
+        <v>1234567890</v>
+      </c>
+      <c r="CG3" s="12">
+        <v>20122009</v>
+      </c>
+      <c r="CH3" s="12">
+        <v>123456789</v>
+      </c>
+      <c r="CI3" s="12">
+        <v>98</v>
+      </c>
+      <c r="CJ3" s="12">
+        <v>123</v>
+      </c>
+      <c r="CK3" s="11">
+        <v>123</v>
+      </c>
+      <c r="CL3" s="11">
+        <v>1234567899</v>
+      </c>
+      <c r="CM3" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="CN3" s="11">
+        <v>8465498615</v>
+      </c>
+      <c r="CO3" s="11">
+        <v>12345678912345</v>
+      </c>
+      <c r="CP3" s="11">
+        <v>123456789</v>
+      </c>
+      <c r="CQ3" s="11">
+        <v>987654321</v>
+      </c>
+      <c r="CR3" s="11">
+        <v>123456789</v>
+      </c>
+      <c r="CS3" s="11">
+        <v>123456789</v>
+      </c>
+      <c r="CT3" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="CU3" s="10" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="4" spans="1:99">
       <c r="A4" s="9">
@@ -1679,6 +1895,97 @@
       <c r="AZ4" s="10" t="s">
         <v>144</v>
       </c>
+      <c r="BA4" s="12">
+        <v>123</v>
+      </c>
+      <c r="BB4" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="BC4" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="BD4" s="11"/>
+      <c r="BE4" s="11"/>
+      <c r="BF4" s="11"/>
+      <c r="BG4" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="BH4" s="10">
+        <v>1234</v>
+      </c>
+      <c r="BI4" s="11">
+        <v>123</v>
+      </c>
+      <c r="BJ4" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="BK4" s="11">
+        <v>567</v>
+      </c>
+      <c r="BL4" s="11"/>
+      <c r="BM4" s="11"/>
+      <c r="BN4" s="11">
+        <v>22112022</v>
+      </c>
+      <c r="BO4" s="10">
+        <v>3072023</v>
+      </c>
+      <c r="BP4" s="11"/>
+      <c r="BQ4" s="10"/>
+      <c r="BR4" s="11">
+        <v>5678</v>
+      </c>
+      <c r="BS4" s="11"/>
+      <c r="BT4" s="11"/>
+      <c r="BU4" s="11"/>
+      <c r="BV4" s="10">
+        <v>9876</v>
+      </c>
+      <c r="BW4" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="BX4" s="10"/>
+      <c r="BY4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="BZ4" s="10">
+        <v>4</v>
+      </c>
+      <c r="CA4" s="10"/>
+      <c r="CB4" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="CC4" s="10"/>
+      <c r="CD4" s="12"/>
+      <c r="CE4" s="11">
+        <v>123</v>
+      </c>
+      <c r="CF4" s="12">
+        <v>12345</v>
+      </c>
+      <c r="CG4" s="12">
+        <v>16012025</v>
+      </c>
+      <c r="CH4" s="12"/>
+      <c r="CI4" s="12"/>
+      <c r="CJ4" s="12">
+        <v>456</v>
+      </c>
+      <c r="CK4" s="11"/>
+      <c r="CL4" s="11"/>
+      <c r="CM4" s="10"/>
+      <c r="CN4" s="11">
+        <v>65452543120651</v>
+      </c>
+      <c r="CO4" s="11"/>
+      <c r="CP4" s="11"/>
+      <c r="CQ4" s="11"/>
+      <c r="CR4" s="11"/>
+      <c r="CS4" s="11"/>
+      <c r="CT4" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="CU4" s="10"/>
     </row>
     <row r="5" spans="1:99">
       <c r="A5" s="9">
@@ -1747,6 +2054,55 @@
       <c r="AX5" s="10"/>
       <c r="AY5" s="10"/>
       <c r="AZ5" s="10"/>
+      <c r="BA5" s="12"/>
+      <c r="BB5" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="BC5" s="11"/>
+      <c r="BD5" s="11"/>
+      <c r="BE5" s="11"/>
+      <c r="BF5" s="11"/>
+      <c r="BG5" s="11"/>
+      <c r="BH5" s="10"/>
+      <c r="BI5" s="11"/>
+      <c r="BJ5" s="11"/>
+      <c r="BK5" s="11">
+        <v>8910</v>
+      </c>
+      <c r="BL5" s="11"/>
+      <c r="BM5" s="11"/>
+      <c r="BN5" s="11"/>
+      <c r="BO5" s="10"/>
+      <c r="BP5" s="11"/>
+      <c r="BQ5" s="10"/>
+      <c r="BR5" s="11">
+        <v>123456789</v>
+      </c>
+      <c r="BS5" s="11"/>
+      <c r="BT5" s="11"/>
+      <c r="BU5" s="11"/>
+      <c r="BV5" s="10"/>
+      <c r="BW5" s="11"/>
+      <c r="BX5" s="10"/>
+      <c r="BY5" s="10"/>
+      <c r="BZ5" s="10"/>
+      <c r="CA5" s="10"/>
+      <c r="CB5" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="CC5" s="10"/>
+      <c r="CD5" s="12"/>
+      <c r="CE5" s="11"/>
+      <c r="CF5" s="12"/>
+      <c r="CG5" s="12"/>
+      <c r="CH5" s="12"/>
+      <c r="CI5" s="12"/>
+      <c r="CJ5" s="12">
+        <v>8</v>
+      </c>
+      <c r="CK5" s="11"/>
+      <c r="CL5" s="11"/>
+      <c r="CM5" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Formato PF finalizado temporalmente
</commit_message>
<xml_diff>
--- a/FormatoPF.xlsx
+++ b/FormatoPF.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="184">
   <si>
     <t>E N C A B E Z A D O</t>
   </si>
@@ -316,10 +316,13 @@
     <t>1qds</t>
   </si>
   <si>
+    <t>28042003</t>
+  </si>
+  <si>
     <t>si</t>
   </si>
   <si>
-    <t>1234567890111</t>
+    <t>Valadez</t>
   </si>
   <si>
     <t>niña</t>
@@ -331,6 +334,9 @@
     <t>Luz</t>
   </si>
   <si>
+    <t>01012003</t>
+  </si>
+  <si>
     <t>dsa</t>
   </si>
   <si>
@@ -352,6 +358,9 @@
     <t>clave1</t>
   </si>
   <si>
+    <t>30061976</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
@@ -385,6 +394,9 @@
     <t>Guan</t>
   </si>
   <si>
+    <t>13122017</t>
+  </si>
+  <si>
     <t>f</t>
   </si>
   <si>
@@ -427,6 +439,12 @@
     <t>Si</t>
   </si>
   <si>
+    <t>25122018</t>
+  </si>
+  <si>
+    <t>20112005</t>
+  </si>
+  <si>
     <t>dos</t>
   </si>
   <si>
@@ -445,6 +463,9 @@
     <t>Guardia</t>
   </si>
   <si>
+    <t>11062017</t>
+  </si>
+  <si>
     <t>Brasil</t>
   </si>
   <si>
@@ -470,6 +491,18 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>05112023</t>
+  </si>
+  <si>
+    <t>18032024</t>
+  </si>
+  <si>
+    <t>29092022</t>
+  </si>
+  <si>
+    <t>07082023</t>
   </si>
   <si>
     <t>ABCDEFG12345kkkkkkkkkkkkkkkkkk
@@ -492,6 +525,12 @@
     <t>nombre1</t>
   </si>
   <si>
+    <t>27042006</t>
+  </si>
+  <si>
+    <t>20122009</t>
+  </si>
+  <si>
     <t>correo@gmail.com</t>
   </si>
   <si>
@@ -501,6 +540,12 @@
     <t>fr</t>
   </si>
   <si>
+    <t>22112022</t>
+  </si>
+  <si>
+    <t>03072023</t>
+  </si>
+  <si>
     <t>DE</t>
   </si>
   <si>
@@ -510,6 +555,9 @@
     <t>nombre2</t>
   </si>
   <si>
+    <t>16012025</t>
+  </si>
+  <si>
     <t>name3</t>
   </si>
   <si>
@@ -519,8 +567,9 @@
     <t>Arturo</t>
   </si>
   <si>
-    <t>Mi domicilio muy largo para
-comprobar el salto de linea</t>
+    <t>Mi domicilio muy
+largo para comprobar
+el salto de linea</t>
   </si>
   <si>
     <t>Arturito</t>
@@ -972,7 +1021,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU5"/>
+  <dimension ref="A1:DB5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1076,7 +1125,8 @@
     <col min="96" max="96" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="100" max="106" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:99" s="1" customFormat="1">
@@ -1501,113 +1551,113 @@
       <c r="C3" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="11">
-        <v>28042003</v>
+      <c r="D3" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="11">
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="K3" s="12">
-        <v>1012003</v>
+        <v>105</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="N3" s="10">
         <v>1233</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="P3" s="10">
         <v>5</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="U3" s="10">
         <v>12</v>
       </c>
-      <c r="V3" s="10">
-        <v>30061976</v>
+      <c r="V3" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
       <c r="AB3" s="11" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AD3" s="11">
         <v>12341</v>
       </c>
-      <c r="AE3" s="10">
-        <v>13122017</v>
+      <c r="AE3" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="AF3" s="10">
         <v>1234</v>
       </c>
       <c r="AG3" s="10" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="AH3" s="10">
         <v>12345</v>
       </c>
       <c r="AI3" s="10" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="AJ3" s="12" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="AL3" s="12" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="AM3" s="12" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="AN3" s="12" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="AO3" s="12" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="AP3" s="12">
         <v>123</v>
@@ -1622,46 +1672,46 @@
         <v>12345678901</v>
       </c>
       <c r="AT3" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="AU3" s="10">
-        <v>25122018</v>
+        <v>140</v>
+      </c>
+      <c r="AU3" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="AV3" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AW3" s="10">
         <v>12345</v>
       </c>
-      <c r="AX3" s="10">
-        <v>20112005</v>
-      </c>
-      <c r="AY3" s="10">
-        <v>20112005</v>
+      <c r="AX3" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="AZ3" s="10" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="BA3" s="12">
         <v>1234567890</v>
       </c>
       <c r="BB3" s="12" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="BC3" s="11" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="BD3" s="11" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="BE3" s="11" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="BF3" s="11" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="BG3" s="11" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="BH3" s="10">
         <v>123456789</v>
@@ -1670,28 +1720,28 @@
         <v>1234</v>
       </c>
       <c r="BJ3" s="11" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="BK3" s="11">
         <v>1234</v>
       </c>
-      <c r="BL3" s="11">
-        <v>5112023</v>
-      </c>
-      <c r="BM3" s="11">
-        <v>18032024</v>
-      </c>
-      <c r="BN3" s="11">
-        <v>29092022</v>
-      </c>
-      <c r="BO3" s="10">
-        <v>7082023</v>
-      </c>
-      <c r="BP3" s="11">
-        <v>5112023</v>
+      <c r="BL3" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="BM3" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN3" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO3" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="BP3" s="11" t="s">
+        <v>159</v>
       </c>
       <c r="BQ3" s="10" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="BR3" s="11">
         <v>1234</v>
@@ -1709,13 +1759,13 @@
         <v>1234</v>
       </c>
       <c r="BW3" s="11" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="BX3" s="10" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="BY3" s="10" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="BZ3" s="10">
         <v>123</v>
@@ -1724,13 +1774,13 @@
         <v>1234567890</v>
       </c>
       <c r="CB3" s="10" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="CC3" s="10">
         <v>1234567890</v>
       </c>
-      <c r="CD3" s="12">
-        <v>27042006</v>
+      <c r="CD3" s="12" t="s">
+        <v>168</v>
       </c>
       <c r="CE3" s="11">
         <v>1234567890</v>
@@ -1738,8 +1788,8 @@
       <c r="CF3" s="12">
         <v>1234567890</v>
       </c>
-      <c r="CG3" s="12">
-        <v>20122009</v>
+      <c r="CG3" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="CH3" s="12">
         <v>123456789</v>
@@ -1757,7 +1807,7 @@
         <v>1234567899</v>
       </c>
       <c r="CM3" s="10" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="CN3" s="11">
         <v>8465498615</v>
@@ -1778,10 +1828,10 @@
         <v>123456789</v>
       </c>
       <c r="CT3" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="CU3" s="10" t="s">
-        <v>166</v>
+        <v>181</v>
+      </c>
+      <c r="CU3" s="11" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:99">
@@ -1789,7 +1839,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
@@ -1798,19 +1848,19 @@
         <v>4</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="10" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="N4" s="10">
         <v>456</v>
@@ -1821,24 +1871,24 @@
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
       <c r="X4" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="Z4" s="11"/>
       <c r="AA4" s="11"/>
       <c r="AB4" s="11" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AD4" s="11"/>
       <c r="AE4" s="10"/>
@@ -1850,21 +1900,21 @@
         <v>21</v>
       </c>
       <c r="AI4" s="10" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="AJ4" s="12" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="AK4" s="12"/>
       <c r="AL4" s="12"/>
       <c r="AM4" s="12" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="AN4" s="12" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="AO4" s="12" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="AP4" s="12">
         <v>12345</v>
@@ -1879,13 +1929,13 @@
         <v>123</v>
       </c>
       <c r="AT4" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="AU4" s="10">
-        <v>11062017</v>
+        <v>148</v>
+      </c>
+      <c r="AU4" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="AV4" s="10" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="AW4" s="10">
         <v>12345</v>
@@ -1893,22 +1943,22 @@
       <c r="AX4" s="10"/>
       <c r="AY4" s="10"/>
       <c r="AZ4" s="10" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="BA4" s="12">
         <v>123</v>
       </c>
       <c r="BB4" s="12" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="BC4" s="11" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="BD4" s="11"/>
       <c r="BE4" s="11"/>
       <c r="BF4" s="11"/>
       <c r="BG4" s="11" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="BH4" s="10">
         <v>1234</v>
@@ -1917,18 +1967,18 @@
         <v>123</v>
       </c>
       <c r="BJ4" s="11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="BK4" s="11">
         <v>567</v>
       </c>
       <c r="BL4" s="11"/>
       <c r="BM4" s="11"/>
-      <c r="BN4" s="11">
-        <v>22112022</v>
-      </c>
-      <c r="BO4" s="10">
-        <v>3072023</v>
+      <c r="BN4" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="BO4" s="10" t="s">
+        <v>174</v>
       </c>
       <c r="BP4" s="11"/>
       <c r="BQ4" s="10"/>
@@ -1942,18 +1992,18 @@
         <v>9876</v>
       </c>
       <c r="BW4" s="11" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="BX4" s="10"/>
       <c r="BY4" s="10" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="BZ4" s="10">
         <v>4</v>
       </c>
       <c r="CA4" s="10"/>
       <c r="CB4" s="10" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="CC4" s="10"/>
       <c r="CD4" s="12"/>
@@ -1963,8 +2013,8 @@
       <c r="CF4" s="12">
         <v>12345</v>
       </c>
-      <c r="CG4" s="12">
-        <v>16012025</v>
+      <c r="CG4" s="12" t="s">
+        <v>178</v>
       </c>
       <c r="CH4" s="12"/>
       <c r="CI4" s="12"/>
@@ -1983,9 +2033,9 @@
       <c r="CR4" s="11"/>
       <c r="CS4" s="11"/>
       <c r="CT4" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="CU4" s="10"/>
+        <v>183</v>
+      </c>
+      <c r="CU4" s="11"/>
     </row>
     <row r="5" spans="1:99">
       <c r="A5" s="9">
@@ -1997,7 +2047,7 @@
       <c r="E5" s="10"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="10"/>
@@ -2016,16 +2066,16 @@
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
       <c r="X5" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AD5" s="11"/>
       <c r="AE5" s="10"/>
@@ -2056,7 +2106,7 @@
       <c r="AZ5" s="10"/>
       <c r="BA5" s="12"/>
       <c r="BB5" s="12" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="BC5" s="11"/>
       <c r="BD5" s="11"/>
@@ -2088,7 +2138,7 @@
       <c r="BZ5" s="10"/>
       <c r="CA5" s="10"/>
       <c r="CB5" s="10" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="CC5" s="10"/>
       <c r="CD5" s="12"/>
@@ -2103,6 +2153,14 @@
       <c r="CK5" s="11"/>
       <c r="CL5" s="11"/>
       <c r="CM5" s="10"/>
+      <c r="CN5" s="11"/>
+      <c r="CO5" s="11"/>
+      <c r="CP5" s="11"/>
+      <c r="CQ5" s="11"/>
+      <c r="CR5" s="11"/>
+      <c r="CS5" s="11"/>
+      <c r="CT5" s="11"/>
+      <c r="CU5" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Avance de simplificacion de codigo
</commit_message>
<xml_diff>
--- a/FormatoPF.xlsx
+++ b/FormatoPF.xlsx
@@ -1021,7 +1021,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DB5"/>
+  <dimension ref="A1:DB6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2162,6 +2162,109 @@
       <c r="CT5" s="11"/>
       <c r="CU5" s="11"/>
     </row>
+    <row r="6" spans="1:99">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="12"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="12"/>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="12"/>
+      <c r="AO6" s="12"/>
+      <c r="AP6" s="12"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="12"/>
+      <c r="BB6" s="12"/>
+      <c r="BC6" s="11"/>
+      <c r="BD6" s="11"/>
+      <c r="BE6" s="11"/>
+      <c r="BF6" s="11"/>
+      <c r="BG6" s="11"/>
+      <c r="BH6" s="10"/>
+      <c r="BI6" s="11"/>
+      <c r="BJ6" s="11"/>
+      <c r="BK6" s="11"/>
+      <c r="BL6" s="11"/>
+      <c r="BM6" s="11"/>
+      <c r="BN6" s="11"/>
+      <c r="BO6" s="10"/>
+      <c r="BP6" s="11"/>
+      <c r="BQ6" s="10"/>
+      <c r="BR6" s="11"/>
+      <c r="BS6" s="11"/>
+      <c r="BT6" s="11"/>
+      <c r="BU6" s="11"/>
+      <c r="BV6" s="10"/>
+      <c r="BW6" s="11"/>
+      <c r="BX6" s="10"/>
+      <c r="BY6" s="10"/>
+      <c r="BZ6" s="10"/>
+      <c r="CA6" s="10"/>
+      <c r="CB6" s="10"/>
+      <c r="CC6" s="10"/>
+      <c r="CD6" s="12"/>
+      <c r="CE6" s="11"/>
+      <c r="CF6" s="12"/>
+      <c r="CG6" s="12"/>
+      <c r="CH6" s="12"/>
+      <c r="CI6" s="12"/>
+      <c r="CJ6" s="12"/>
+      <c r="CK6" s="11"/>
+      <c r="CL6" s="11"/>
+      <c r="CM6" s="10"/>
+      <c r="CN6" s="11"/>
+      <c r="CO6" s="11"/>
+      <c r="CP6" s="11"/>
+      <c r="CQ6" s="11"/>
+      <c r="CR6" s="11"/>
+      <c r="CS6" s="11"/>
+      <c r="CT6" s="11"/>
+      <c r="CU6" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:F1"/>

</xml_diff>

<commit_message>
Codigo corregido de detalles pequeños
</commit_message>
<xml_diff>
--- a/FormatoPF.xlsx
+++ b/FormatoPF.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="188">
   <si>
     <t>E N C A B E Z A D O</t>
   </si>
@@ -454,7 +454,7 @@
     <t>20112005</t>
   </si>
   <si>
-    <t>dos</t>
+    <t>do</t>
   </si>
   <si>
     <t>name2</t>
@@ -478,7 +478,7 @@
     <t>Brasil</t>
   </si>
   <si>
-    <t>tres</t>
+    <t>tr</t>
   </si>
   <si>
     <t>name1</t>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>nombre3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Arturo</t>
@@ -1135,10 +1138,11 @@
     <col min="97" max="97" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="100" max="106" width="9.140625" style="1"/>
+    <col min="100" max="100" width="1.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="101" max="106" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" s="1" customFormat="1">
+    <row r="1" spans="1:100" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1255,7 @@
       <c r="CT1" s="3"/>
       <c r="CU1" s="3"/>
     </row>
-    <row r="2" spans="1:99">
+    <row r="2" spans="1:100">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1550,7 +1554,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:99">
+    <row r="3" spans="1:100">
       <c r="A3" s="9">
         <v>13</v>
       </c>
@@ -1612,7 +1616,7 @@
         <v>114</v>
       </c>
       <c r="U3" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>115</v>
@@ -1843,13 +1847,16 @@
         <v>123456789</v>
       </c>
       <c r="CT3" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="CU3" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="CV3" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="CU3" s="11" t="s">
-        <v>185</v>
-      </c>
     </row>
-    <row r="4" spans="1:99">
+    <row r="4" spans="1:100">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -2050,11 +2057,14 @@
       <c r="CR4" s="11"/>
       <c r="CS4" s="11"/>
       <c r="CT4" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CU4" s="11"/>
+      <c r="CV4" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
-    <row r="5" spans="1:99">
+    <row r="5" spans="1:100">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -2178,8 +2188,11 @@
       <c r="CS5" s="11"/>
       <c r="CT5" s="11"/>
       <c r="CU5" s="11"/>
+      <c r="CV5" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
-    <row r="6" spans="1:99">
+    <row r="6" spans="1:100">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -2281,6 +2294,9 @@
       <c r="CS6" s="11"/>
       <c r="CT6" s="11"/>
       <c r="CU6" s="11"/>
+      <c r="CV6" s="1" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Cambiar a tipo float datos con decimales
</commit_message>
<xml_diff>
--- a/FormatoPF.xlsx
+++ b/FormatoPF.xlsx
@@ -1700,7 +1700,7 @@
         <v>110</v>
       </c>
       <c r="AW3" s="10">
-        <v>12345</v>
+        <v>12345.22</v>
       </c>
       <c r="AX3" s="10" t="s">
         <v>145</v>
@@ -1742,7 +1742,7 @@
         <v>161</v>
       </c>
       <c r="BK3" s="11">
-        <v>1234</v>
+        <v>1234.5</v>
       </c>
       <c r="BL3" s="11" t="s">
         <v>162</v>
@@ -1763,13 +1763,13 @@
         <v>166</v>
       </c>
       <c r="BR3" s="11">
-        <v>1234</v>
+        <v>1234.7</v>
       </c>
       <c r="BS3" s="11">
-        <v>1234567890</v>
+        <v>1234567.4</v>
       </c>
       <c r="BT3" s="11">
-        <v>123456789</v>
+        <v>12345.24</v>
       </c>
       <c r="BU3" s="11">
         <v>123456789</v>
@@ -1811,7 +1811,7 @@
         <v>172</v>
       </c>
       <c r="CH3" s="12">
-        <v>123456789</v>
+        <v>12345.3</v>
       </c>
       <c r="CI3" s="12">
         <v>98</v>
@@ -1823,7 +1823,7 @@
         <v>12345</v>
       </c>
       <c r="CL3" s="11">
-        <v>1234567899</v>
+        <v>1234567.7</v>
       </c>
       <c r="CM3" s="10" t="s">
         <v>173</v>
@@ -1962,7 +1962,7 @@
         <v>153</v>
       </c>
       <c r="AW4" s="10">
-        <v>123456789</v>
+        <v>123456.8</v>
       </c>
       <c r="AX4" s="10"/>
       <c r="AY4" s="10"/>
@@ -1994,7 +1994,7 @@
         <v>112</v>
       </c>
       <c r="BK4" s="11">
-        <v>567</v>
+        <v>567.66</v>
       </c>
       <c r="BL4" s="11"/>
       <c r="BM4" s="11"/>
@@ -2007,11 +2007,13 @@
       <c r="BP4" s="11"/>
       <c r="BQ4" s="10"/>
       <c r="BR4" s="11">
-        <v>5678</v>
+        <v>5678.78</v>
       </c>
       <c r="BS4" s="11"/>
       <c r="BT4" s="11"/>
-      <c r="BU4" s="11"/>
+      <c r="BU4" s="11">
+        <v>75.2</v>
+      </c>
       <c r="BV4" s="10">
         <v>9876</v>
       </c>
@@ -2032,10 +2034,10 @@
       <c r="CC4" s="10"/>
       <c r="CD4" s="12"/>
       <c r="CE4" s="11">
-        <v>123</v>
+        <v>123.2</v>
       </c>
       <c r="CF4" s="12">
-        <v>12345</v>
+        <v>12345.7</v>
       </c>
       <c r="CG4" s="12" t="s">
         <v>181</v>
@@ -2144,7 +2146,7 @@
       <c r="BI5" s="11"/>
       <c r="BJ5" s="11"/>
       <c r="BK5" s="11">
-        <v>8910</v>
+        <v>8910.549999999999</v>
       </c>
       <c r="BL5" s="11"/>
       <c r="BM5" s="11"/>

</xml_diff>